<commit_message>
Update summary report in Excel format with latest data
</commit_message>
<xml_diff>
--- a/reports/summary.xlsx
+++ b/reports/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,105 +508,105 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HP-  OmniBook 5 Flip 2 - in - 1 14" 2K Touch - Screen Laptop  -  Intel Core 7  -  16GB Memory  -  512GB SSD  -  Glacier Silver</t>
+          <t>Dell-  Inspiron 15" Touch Screen Laptop  -  Intel Core i7 with 16GB Memory  -  1TB SSD  -  Black</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.bestbuy.com/site/hp-omnibook-5-flip-2-in-1-14-2k-touch-screen-laptop-intel-core-7-16gb-memory-512gb-ssd-glacier-silver/6614107.p?skuId=6614107</t>
+          <t>https://www.bestbuy.com/site/dell-inspiron-15-touch-screen-laptop-intel-core-i7-with-16gb-memory-1tb-ssd-black/6610571.p?skuId=6610571</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$549.99</t>
+          <t>$649.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rating 4.8 out of 5 stars with 19 reviews</t>
+          <t>Rating 4.6 out of 5 stars with 81 reviews</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>6614107</t>
+          <t>6610571</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>14-fp0023dx</t>
+          <t>i3530-7728BLK-PUS</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lenovo-  Yoga 7 2 - in - 1  -  Copilot+ PC  -  16" 2K LCD Touchscreen Laptop  -  AMD Ryzen AI 5 340  -  16GB Memory  -  512GB SSD  -  Seashell</t>
+          <t>Dell-  Inspiron 15" Touch Screen Laptop  -  Intel Core i5 with 8GB Memory  -  512GB SSD  -  Black</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.bestbuy.com/site/lenovo-yoga-7-2-in-1-copilot-pc-16-2k-lcd-touchscreen-laptop-amd-ryzen-ai-5-340-16gb-memory-512gb-ssd-seashell/6615774.p?skuId=6615774</t>
+          <t>https://www.bestbuy.com/site/dell-inspiron-15-touch-screen-laptop-intel-core-i5-with-8gb-memory-512gb-ssd-black/6610570.p?skuId=6610570</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$549.99</t>
+          <t>$629.99</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rating 5 out of 5 stars with 3 reviews</t>
+          <t>Rating 4.7 out of 5 stars with 118 reviews</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>6615774</t>
+          <t>6610570</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>83JU0001US</t>
+          <t>i3530-5623BLK-PUS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HP-  OmniBook 5 Flip 2 - in - 1 14" 2K Touch - Screen Laptop  -  Intel Core 5  -  8GB Memory  -  512GB SSD  -  Glacier Silver</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.bestbuy.com/site/hp-omnibook-5-flip-2-in-1-14-2k-touch-screen-laptop-intel-core-5-8gb-memory-512gb-ssd-glacier-silver/6614109.p?skuId=6614109</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$699.99</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Rating 4.8 out of 5 stars with 79 reviews</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>6614109</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>14-fp0013dx</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1235,6 +1235,41 @@
         </is>
       </c>
       <c r="G23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>

<commit_message>
Update summary report with latest data
</commit_message>
<xml_diff>
--- a/reports/summary.xlsx
+++ b/reports/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,490 +473,518 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dell-  Inspiron 15" Touch Screen Laptop  -  Intel Core i5 with 8GB Memory  -  512GB SSD  -  Black</t>
+          <t>Lenovo-  Yoga 7i 2 - in - 1  -  Copilot+ PC  -  16" 2K Touchscreen Laptop  -  Intel Core Ultra 5 Processor  -  16GB Memory  -  512GB SSD  -  Luna Grey</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.bestbuy.com/site/dell-inspiron-15-touch-screen-laptop-intel-core-i5-with-8gb-memory-512gb-ssd-black/6610570.p?skuId=6610570</t>
+          <t>https://www.bestbuy.com/site/lenovo-yoga-7i-2-in-1-copilot-pc-16-2k-touchscreen-laptop-intel-core-ultra-5-processor-16gb-memory-512gb-ssd-luna-grey/6615769.p?skuId=6615769</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$629.99</t>
+          <t>$649.99</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rating 4.7 out of 5 stars with 118 reviews</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>118</v>
+          <t>Rating 4.9 out of 5 stars with 7 reviews</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6610570</t>
+          <t>6615769</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>i3530-5623BLK-PUS</t>
+          <t>83JT0000US</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dell-  Inspiron 15" Touch Screen Laptop  -  Intel Core i7 with 16GB Memory  -  1TB SSD  -  Black</t>
+          <t>HP-  OmniBook 5 Flip 2 - in - 1 14" 2K Touch - Screen Laptop  -  Intel Core 7  -  16GB Memory  -  512GB SSD  -  Glacier Silver</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.bestbuy.com/site/dell-inspiron-15-touch-screen-laptop-intel-core-i7-with-16gb-memory-1tb-ssd-black/6610571.p?skuId=6610571</t>
+          <t>https://www.bestbuy.com/site/hp-omnibook-5-flip-2-in-1-14-2k-touch-screen-laptop-intel-core-7-16gb-memory-512gb-ssd-glacier-silver/6614107.p?skuId=6614107</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$649.99</t>
+          <t>$549.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rating 4.6 out of 5 stars with 81 reviews</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>81</v>
+          <t>Rating 4.8 out of 5 stars with 19 reviews</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>6610571</t>
+          <t>6614107</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>i3530-7728BLK-PUS</t>
+          <t>14-fp0023dx</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dell-  Inspiron 15" Touch Screen Laptop  -  Intel Core i5 with 8GB Memory  -  512GB SSD  -  Black</t>
+          <t>Lenovo-  Yoga 9i 2 - in - 1 14" 2.8K OLED Touchscreen Laptop with Pen  -  Intel Core Ultra 7 155H with 16GB Memory  -  1TB SSD  -  Cosmic Blue</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.bestbuy.com/site/dell-inspiron-15-touch-screen-laptop-intel-core-i5-with-8gb-memory-512gb-ssd-black/6610570.p?skuId=6610570</t>
+          <t>https://www.bestbuy.com/site/lenovo-yoga-9i-2-in-1-14-2-8k-oled-touchscreen-laptop-with-pen-intel-core-ultra-7-155h-with-16gb-memory-1tb-ssd-cosmic-blue/6571371.p?skuId=6571371</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$629.99</t>
+          <t>$999.99</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rating 4.7 out of 5 stars with 118 reviews</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>118</v>
+          <t>Rating 4.4 out of 5 stars with 222 reviews</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>6610570</t>
+          <t>6571371</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>i3530-5623BLK-PUS</t>
+          <t>83AC0001US</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  17.3" Full HD Laptop  -  AMD Ryzen 5  -  8GB Memory  -  512GB SSD  -  Natural Silver</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-17-3-full-hd-laptop-amd-ryzen-5-8gb-memory-512gb-ssd-natural-silver/6612252.p?skuId=6612252</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$629.99</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
+          <t>Rating 4.7 out of 5 stars with 216 reviews</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>216</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6612252</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>17-cp2025dx</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  Victus 15.6" 144Hz Full HD Gaming Laptop  -  Intel Core i5  -  8GB Memory  -  NVIDIA GeForce RTX 3050  -  512GB SSD  -  Mica Silver</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-victus-15-6-144hz-full-hd-gaming-laptop-intel-core-i5-8gb-memory-nvidia-geforce-rtx-3050-512gb-ssd-mica-silver/6618924.p?skuId=6618924</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$529.99</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
+          <t>Rating 4.5 out of 5 stars with 50 reviews</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6618924</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>15-fa2013dx</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Lenovo-  Yoga 7i 2 - in - 1  -  Copilot+ PC  -  14" 2K OLED Touchscreen Laptop  -  Intel Core Ultra 7 Processor  -  16GB Memory  -  1TB SSD  -  Luna Grey</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/lenovo-yoga-7i-2-in-1-copilot-pc-14-2k-oled-touchscreen-laptop-intel-core-ultra-7-processor-16gb-memory-1tb-ssd-luna-grey/6615777.p?skuId=6615777</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$799.99</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
+          <t>Rating 5 out of 5 stars with 1 reviewfalse</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6615777</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>83JQ000KUS</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  14" Refurbished 1920 x 1080 FHD  -  Intel 11th Gen Core i5 - 1145G7 with 32GB RAM  -  Intel Iris Xe Graphics  -  1TB SSD  -  Silver</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-14-refurbished-1920-x-1080-fhd-intel-11th-gen-core-i5-1145g7-with-32gb-ram-intel-iris-xe-graphics-1tb-ssd-silver/6545476.p?skuId=6545476</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$666.99</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
+          <t>Rating 5 out of 5 stars with 1 reviewfalse</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6545476</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>840 G8</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  ZBook 15U G5 15.6" Refurbished Laptop  -  Intel 8th Gen Core i7 with 32GB Memory  -  Intel UHD Graphics 620  -  512GB SSD  -  Silver</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-zbook-15u-g5-15-6-refurbished-laptop-intel-8th-gen-core-i7-with-32gb-memory-intel-uhd-graphics-620-512gb-ssd-silver/6579728.p?skuId=6579728</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$643.99</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
+          <t>Not yet reviewed</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Not yet reviewed</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6579728</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>ZBook 15U G5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  ProBook 440 G11 14" IPS 1920 x 1200 (WUXGA) Laptop  -  Intel Core Ultra 5 with 16GB Memory  -  256 GB SSD  -  Pike Silver, Silver</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-probook-440-g11-14-ips-1920-x-1200-wuxga-laptop-intel-core-ultra-5-with-16gb-memory-256-gb-ssd-pike-silver-silver/6588386.p?skuId=6588386</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1,089.99</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
+          <t>Not yet reviewed</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Not yet reviewed</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6588386</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A1LC2UT#ABA</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  Envy 2 - in - 1 16" 2K Touch - Screen Laptop  -  AMD Ryzen 7  -  16GB Memory  -  1TB SSD  -  Meteor Silver</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-envy-2-in-1-16-2k-touch-screen-laptop-amd-ryzen-7-16gb-memory-1tb-ssd-meteor-silver/6571083.p?skuId=6571083</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$760.99</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
+          <t>Rating 4.7 out of 5 stars with 790 reviews</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>790</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6571083</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>16-ad0023dx/9S1M4UA#ABA</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  OmniBook Ultra Flip  -  Copilot+ PC  -  14" 3K OLED Touch - Screen Laptop  -  Intel Core Ultra 7  -  16GB Memory  -  1TB SSD  -  Eclipse Grey</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-omnibook-ultra-flip-copilot-pc-14-3k-oled-touch-screen-laptop-intel-core-ultra-7-16gb-memory-1tb-ssd-eclipse-grey/6593552.p?skuId=6593552</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1,199.99</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
+          <t>Rating 4.5 out of 5 stars with 155 reviews</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6593552</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>14-fh0013dx/A9SR3UA#ABA</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  Envy 2 - in - 1 16" 2K Touch - Screen Laptop  -  Intel Core Ultra 7  -  16GB Memory  -  1TB SSD  -  Glacier Silver</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-envy-2-in-1-16-2k-touch-screen-laptop-intel-core-ultra-7-16gb-memory-1tb-ssd-glacier-silver/6571084.p?skuId=6571084</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$760.99</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
+          <t>Rating 4.7 out of 5 stars with 1275 reviews</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1,275</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6571084</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>16-ac0023dx/9S1R6UA#ABA</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  Envy 2 - in - 1 14" 2K Touch - Screen Laptop  -  Intel Core Ultra 7  -  16GB Memory  -  1TB SSD  -  Meteor Silver</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-envy-2-in-1-14-2k-touch-screen-laptop-intel-core-ultra-7-16gb-memory-1tb-ssd-meteor-silver/6571085.p?skuId=6571085</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$701.99</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
+          <t>Rating 4.7 out of 5 stars with 569 reviews</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>569</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6571085</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>14-fc0023dx/9T8G4UA#ABA</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HP-  Envy 2 - in - 1 16" 2K Touch - Screen Laptop  -  Intel Core Ultra 5  -  16GB Memory  -  512GB SSD  -  Glacier Silver</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/hp-envy-2-in-1-16-2k-touch-screen-laptop-intel-core-ultra-5-16gb-memory-512gb-ssd-glacier-silver/6571081.p?skuId=6571081</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$617.99</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
+          <t>Rating 4.7 out of 5 stars with 525 reviews</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>525</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6571081</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>16-ac0013dx/9S1R5UA#ABA</t>
         </is>
       </c>
     </row>
@@ -981,8 +1009,10 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1016,8 +1046,10 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1051,8 +1083,10 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1086,8 +1120,10 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1121,8 +1157,10 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="E20" t="n">
-        <v>0</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1138,140 +1176,37 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Lenovo-  Yoga 7i 2 - in - 1 16" 2K Touchscreen Laptop  -  Intel Core Ultra 7 155U with 16GB Memory  -  1TB SSD  -  Storm Grey</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.bestbuy.com/site/lenovo-yoga-7i-2-in-1-16-2k-touchscreen-laptop-intel-core-ultra-7-155u-with-16gb-memory-1tb-ssd-storm-grey/6571369.p?skuId=6571369</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1,049.99</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
+          <t>Rating 4.7 out of 5 stars with 1609 reviews</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1,609</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>6571369</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>N/A</t>
+          <t>83DL0002US</t>
         </is>
       </c>
     </row>

</xml_diff>